<commit_message>
Update descriptors cho Caltech va SUN
Update codebook 10K va pyramid 1x1, 2x2
Scale ma tran U ve [-1 1]
</commit_message>
<xml_diff>
--- a/KetquatrenCaltech256 (Autosaved) (Autosaved) (Autosaved).xlsx
+++ b/KetquatrenCaltech256 (Autosaved) (Autosaved) (Autosaved).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="390" windowWidth="15120" windowHeight="7125" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="390" windowWidth="15120" windowHeight="7125" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Flat" sheetId="1" r:id="rId1"/>
@@ -13,18 +13,18 @@
     <sheet name="Kehoach2014" sheetId="7" r:id="rId4"/>
     <sheet name="eigenclass" sheetId="13" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="16" r:id="rId6"/>
-    <sheet name="ILSVRC_new" sheetId="19" r:id="rId7"/>
-    <sheet name="Caltech256_(1)" sheetId="21" r:id="rId8"/>
-    <sheet name="Caltech256_new" sheetId="17" r:id="rId9"/>
-    <sheet name="report" sheetId="20" r:id="rId10"/>
+    <sheet name="SUN_new" sheetId="22" r:id="rId7"/>
+    <sheet name="ILSVRC_new" sheetId="19" r:id="rId8"/>
+    <sheet name="Caltech256_(1)" sheetId="21" r:id="rId9"/>
+    <sheet name="Caltech256_new" sheetId="17" r:id="rId10"/>
+    <sheet name="report" sheetId="20" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="323">
   <si>
     <t>Tỉ lệ train/val/test: 50%-25%-25%</t>
   </si>
@@ -837,9 +837,6 @@
     <t>0.0190    0.0239    0.0457    0.0604    0.0851    0.0985    0.1071    0.1133    0.1178    0.1213    0.1239    0.1263    0.1286</t>
   </si>
   <si>
-    <t>8.33% 10.08% 14.55% 16.30% 18.25% 18.99% 19.44% 19.82% 20.06% 20.26% 20.41% 20.62% 20.73%</t>
-  </si>
-  <si>
     <t>0.1086    0.1400    0.2051    0.2584    0.3236    0.3529    0.3662    0.3778</t>
   </si>
   <si>
@@ -907,6 +904,97 @@
   </si>
   <si>
     <t>0.1139    0.1441    0.2158    0.2722    0.3438    0.3761    0.3920    0.4067</t>
+  </si>
+  <si>
+    <t>0.0818    0.0994    0.1427    0.1590    0.1788    0.1876    0.1926    0.1959    0.1992    0.2011    0.2033    0.2051    0.2060</t>
+  </si>
+  <si>
+    <t>0.0268    0.0332    0.0612    0.0777    0.1023    0.1144    0.1218    0.1269    0.1306    0.1335    0.1357    0.1376    0.1392</t>
+  </si>
+  <si>
+    <t>0.2294    0.2613    0.3315    0.3878    0.4477    0.4700    0.4822    0.4896</t>
+  </si>
+  <si>
+    <t>0.1139    0.1441    0.2158    0.2722    0.3438    0.3761    0.3919    0.4067</t>
+  </si>
+  <si>
+    <t>0.2294    0.2624    0.3327    0.3896    0.4503    0.4761    0.4878    0.4957</t>
+  </si>
+  <si>
+    <t>0.0915    0.1158    0.1823    0.2403    0.3149    0.3524    0.3713    0.3853</t>
+  </si>
+  <si>
+    <t>0.2289    0.2621    0.3321    0.3896    0.4501    0.4767    0.4886    0.4960</t>
+  </si>
+  <si>
+    <t>0.0984    0.1242    0.1889    0.2464    0.3184    0.3545    0.3728    0.3883</t>
+  </si>
+  <si>
+    <t>0.1354    0.1471    0.1894    0.2211    0.2790    0.2976    0.3088    0.3186</t>
+  </si>
+  <si>
+    <t>22.08% 25.30% 32.62% 37.86% 43.75% 45.99% 47.04% 47.82%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0713    0.0848    0.1162    0.1588    0.2041    0.2252    0.2393    0.2473</t>
+  </si>
+  <si>
+    <t>0.0118    0.0146    0.0296    0.0362    0.0527    0.0603    0.0659    0.0720    0.0743    0.0767    0.0794    0.0815    0.0832</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U scale -1 đến 1 khi train regresser): chưa scale lại sau khi test</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U scale -1 đến 1 khi train regresser):  scale lại sau khi test</t>
+  </si>
+  <si>
+    <t>0.0687    0.0850    0.1259    0.1420    0.1618    0.1700    0.1755    0.1800    0.1834    0.1855    0.1873    0.1896    0.1910</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0260    0.0320    0.0560    0.0695    0.0901    0.1005    0.1071    0.1118    0.1152    0.1178    0.1199    0.1218    0.1233</t>
+  </si>
+  <si>
+    <t>0.2027    0.2349    0.3024    0.3597    0.4155    0.4386    0.4496    0.4549</t>
+  </si>
+  <si>
+    <t>0.0004    0.0005    0.0008    0.0010    0.0012    0.0013    0.0014    0.0014</t>
+  </si>
+  <si>
+    <t>0.2060    0.2421    0.2962    0.3170    0.3668    0.4017    0.4185    0.4283</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1020    0.1267    0.1751    0.1973    0.2521    0.2867    0.3027    0.3123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1691    0.2062    0.2682    0.3260    0.3695    0.3883    0.3967    0.4039
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0004    0.0005    0.0007    0.0009    0.0011    0.0012    0.0013    0.0013</t>
+  </si>
+  <si>
+    <t>App1 ( scale giá trị của ma trận U=U*397  khi train regresser)</t>
+  </si>
+  <si>
+    <t>0.2016    0.2344    0.2894    0.3112    0.3641    0.4007    0.4158    0.4231</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.2046    0.2404    0.2909    0.3088    0.3593    0.3916    0.4064    0.4167</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1010    0.1255    0.1734    0.1954    0.2500    0.2847    0.2996    0.3091</t>
+  </si>
+  <si>
+    <t>0.0833    0.1008    0.1455    0.1630    0.1825    0.1899    0.1944    0.1982    0.2006    0.2026    0.2041    0.2062    0.2073</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.2046    0.2404    0.2909    0.3088    0.3593    0.3916    0.4070    0.4167</t>
+  </si>
+  <si>
+    <t>0.1866    0.2156    0.2704    0.2904    0.3471    0.3858    0.4000    0.4076</t>
+  </si>
+  <si>
+    <t>0.1092    0.1322    0.1767    0.1966    0.2462    0.2753    0.2878    0.2954</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1612,6 +1700,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2249,11 +2344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45439232"/>
-        <c:axId val="45457408"/>
+        <c:axId val="94313856"/>
+        <c:axId val="94332032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45439232"/>
+        <c:axId val="94313856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2263,7 +2358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45457408"/>
+        <c:crossAx val="94332032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2271,7 +2366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45457408"/>
+        <c:axId val="94332032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2282,7 +2377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45439232"/>
+        <c:crossAx val="94313856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2588,11 +2683,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109714432"/>
-        <c:axId val="109744896"/>
+        <c:axId val="100790272"/>
+        <c:axId val="100791808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109714432"/>
+        <c:axId val="100790272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2602,7 +2697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109744896"/>
+        <c:crossAx val="100791808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2610,7 +2705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109744896"/>
+        <c:axId val="100791808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2621,14 +2716,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109714432"/>
+        <c:crossAx val="100790272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3180,11 +3274,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45620608"/>
-        <c:axId val="45634688"/>
+        <c:axId val="94364416"/>
+        <c:axId val="94365952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45620608"/>
+        <c:axId val="94364416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3194,7 +3288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45634688"/>
+        <c:crossAx val="94365952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3202,7 +3296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45634688"/>
+        <c:axId val="94365952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3213,7 +3307,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45620608"/>
+        <c:crossAx val="94364416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3774,11 +3868,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45667072"/>
-        <c:axId val="45668608"/>
+        <c:axId val="99706752"/>
+        <c:axId val="99708288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45667072"/>
+        <c:axId val="99706752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3788,7 +3882,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45668608"/>
+        <c:crossAx val="99708288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3796,7 +3890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45668608"/>
+        <c:axId val="99708288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3807,7 +3901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45667072"/>
+        <c:crossAx val="99706752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4332,11 +4426,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108623744"/>
-        <c:axId val="108625280"/>
+        <c:axId val="99752960"/>
+        <c:axId val="99758848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108623744"/>
+        <c:axId val="99752960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,7 +4440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108625280"/>
+        <c:crossAx val="99758848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4354,7 +4448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108625280"/>
+        <c:axId val="99758848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4365,7 +4459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108623744"/>
+        <c:crossAx val="99752960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4531,11 +4625,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108649472"/>
-        <c:axId val="108655360"/>
+        <c:axId val="99778944"/>
+        <c:axId val="99780480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108649472"/>
+        <c:axId val="99778944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4545,7 +4639,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108655360"/>
+        <c:crossAx val="99780480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4553,7 +4647,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108655360"/>
+        <c:axId val="99780480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4567,7 +4661,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108649472"/>
+        <c:crossAx val="99778944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4941,11 +5035,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109643264"/>
-        <c:axId val="109644800"/>
+        <c:axId val="96594560"/>
+        <c:axId val="100405632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109643264"/>
+        <c:axId val="96594560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4955,7 +5049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109644800"/>
+        <c:crossAx val="100405632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4963,7 +5057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109644800"/>
+        <c:axId val="100405632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4974,13 +5068,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109643264"/>
+        <c:crossAx val="96594560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5010,6 +5105,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5340,11 +5436,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109667456"/>
-        <c:axId val="109668992"/>
+        <c:axId val="100428032"/>
+        <c:axId val="100450304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109667456"/>
+        <c:axId val="100428032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5354,7 +5450,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109668992"/>
+        <c:crossAx val="100450304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5362,7 +5458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109668992"/>
+        <c:axId val="100450304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5373,13 +5469,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109667456"/>
+        <c:crossAx val="100428032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5841,11 +5938,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109704320"/>
-        <c:axId val="109705856"/>
+        <c:axId val="96679808"/>
+        <c:axId val="96681344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109704320"/>
+        <c:axId val="96679808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5855,7 +5952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109705856"/>
+        <c:crossAx val="96681344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5863,7 +5960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109705856"/>
+        <c:axId val="96681344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5874,13 +5971,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109704320"/>
+        <c:crossAx val="96679808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6180,11 +6278,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="109961600"/>
-        <c:axId val="109963136"/>
+        <c:axId val="100746368"/>
+        <c:axId val="100747904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109961600"/>
+        <c:axId val="100746368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6194,7 +6292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109963136"/>
+        <c:crossAx val="100747904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6202,7 +6300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109963136"/>
+        <c:axId val="100747904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6213,14 +6311,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109961600"/>
+        <c:crossAx val="100746368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7057,9 +7154,456 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.44900000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="124" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="124"/>
+      <c r="B4" s="161" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="124"/>
+      <c r="B5" s="161" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="124"/>
+      <c r="B6" s="161" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="124"/>
+      <c r="B7" s="161" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="124"/>
+      <c r="B8" s="161" t="s">
+        <v>305</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="124"/>
+      <c r="B9" s="201" t="s">
+        <v>306</v>
+      </c>
+      <c r="C9" s="161" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="126"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="163" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="B11" s="175" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="E11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="175" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="175" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" s="71" t="s">
+        <v>250</v>
+      </c>
+      <c r="E13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="175" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="174" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="174" t="s">
+        <v>247</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="174" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="185" t="s">
+        <v>248</v>
+      </c>
+      <c r="C18" s="186" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="164" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="165" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="165" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" s="165" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="165" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="165" t="s">
+        <v>214</v>
+      </c>
+      <c r="E21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="164" t="s">
+        <v>207</v>
+      </c>
+      <c r="C22" s="165" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="165" t="s">
+        <v>211</v>
+      </c>
+      <c r="E22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="165" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="167" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" s="165" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="162" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>226</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="166" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="73" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="162" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="73" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="166" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="166" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="73" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" t="s">
+        <v>273</v>
+      </c>
+      <c r="D28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="171" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="171" t="s">
+        <v>279</v>
+      </c>
+      <c r="C30" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="176" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B32" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="176" t="s">
+        <v>260</v>
+      </c>
+      <c r="C35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>263</v>
+      </c>
+      <c r="C39" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3:T6"/>
     </sheetView>
   </sheetViews>
@@ -7071,10 +7615,10 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="45" x14ac:dyDescent="0.25">
@@ -7247,7 +7791,7 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="180" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C6" s="121">
         <v>0.19139999999999999</v>
@@ -7274,7 +7818,7 @@
         <v>0.4395</v>
       </c>
       <c r="L6" s="180" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M6" s="121">
         <v>0.22919999999999999</v>
@@ -7313,7 +7857,7 @@
   <dimension ref="A1:AC24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11496,8 +12040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BE26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J13"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13285,10 +13829,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22:X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13375,7 +13919,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>159</v>
       </c>
@@ -13383,7 +13927,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>161</v>
       </c>
@@ -13391,7 +13935,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
@@ -13399,27 +13943,53 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q22" s="58">
+        <v>0.220786287579921</v>
+      </c>
+      <c r="R22" s="58">
+        <v>0.25302679907495601</v>
+      </c>
+      <c r="S22" s="58">
+        <v>0.32621412052781901</v>
+      </c>
+      <c r="T22" s="58">
+        <v>0.37858794721806599</v>
+      </c>
+      <c r="U22" s="58">
+        <v>0.43749149775540702</v>
+      </c>
+      <c r="V22" s="58">
+        <v>0.45993742347979899</v>
+      </c>
+      <c r="W22" s="58">
+        <v>0.47041218881784802</v>
+      </c>
+      <c r="X22" s="58">
+        <v>0.47816623588627399</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>33</v>
       </c>
@@ -13427,12 +13997,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>176</v>
       </c>
@@ -13474,213 +14044,6 @@
       <c r="B46" t="s">
         <v>180</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="97" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="173">
-        <v>0.20619999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="161" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="124"/>
-      <c r="B5" s="161" t="s">
-        <v>240</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
-      <c r="B6" s="172"/>
-      <c r="C6" s="163"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>32</v>
-      </c>
-      <c r="B7" s="168" t="s">
-        <v>228</v>
-      </c>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="169" t="s">
-        <v>229</v>
-      </c>
-      <c r="C8" s="164" t="s">
-        <v>270</v>
-      </c>
-      <c r="D8" s="165"/>
-      <c r="E8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="168" t="s">
-        <v>230</v>
-      </c>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="169" t="s">
-        <v>231</v>
-      </c>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="170" t="s">
-        <v>232</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="171" t="s">
-        <v>233</v>
-      </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="171" t="s">
-        <v>235</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>268</v>
-      </c>
-      <c r="D14" s="73" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>210</v>
-      </c>
-      <c r="B16" s="164" t="s">
-        <v>206</v>
-      </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="165"/>
-      <c r="E16" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="165" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="165"/>
-      <c r="E17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="164" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="165"/>
-      <c r="E18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="165" t="s">
-        <v>202</v>
-      </c>
-      <c r="C19" s="165"/>
-      <c r="D19" s="165"/>
-      <c r="E19" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="162" t="s">
-        <v>208</v>
-      </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="166" t="s">
-        <v>204</v>
-      </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="162" t="s">
-        <v>209</v>
-      </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="166" t="s">
-        <v>205</v>
-      </c>
-      <c r="C23" s="166"/>
-      <c r="D23" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13688,327 +14051,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.50800000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="124" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" s="95" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="124"/>
-      <c r="B4" s="161" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="62"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="124"/>
-      <c r="B5" s="161" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="62"/>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="124"/>
-      <c r="B6" s="161" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="62"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="124"/>
-      <c r="B7" s="161" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="62"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="126"/>
-      <c r="B8" s="172"/>
-      <c r="C8" s="163"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>32</v>
-      </c>
-      <c r="B9" s="175" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="175" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="175" t="s">
-        <v>230</v>
-      </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="175" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="174" t="s">
-        <v>232</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="174" t="s">
-        <v>247</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="174" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="185" t="s">
-        <v>248</v>
-      </c>
-      <c r="C16" s="186"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>210</v>
-      </c>
-      <c r="B18" s="164" t="s">
-        <v>206</v>
-      </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="165"/>
-      <c r="E18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="165" t="s">
-        <v>203</v>
-      </c>
-      <c r="C19" s="165"/>
-      <c r="D19" s="165"/>
-      <c r="E19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="164" t="s">
-        <v>207</v>
-      </c>
-      <c r="C20" s="165"/>
-      <c r="D20" s="165"/>
-      <c r="E20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
-        <v>202</v>
-      </c>
-      <c r="C21" s="167"/>
-      <c r="D21" s="165"/>
-      <c r="E21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="162" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="166" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="162" t="s">
-        <v>209</v>
-      </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="166" t="s">
-        <v>205</v>
-      </c>
-      <c r="C25" s="166"/>
-      <c r="D25" s="73"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>171</v>
-      </c>
-      <c r="B26" s="171" t="s">
-        <v>205</v>
-      </c>
-      <c r="C26" t="s">
-        <v>292</v>
-      </c>
-      <c r="D26" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="171" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="171" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>279</v>
-      </c>
-      <c r="B29" s="171" t="s">
-        <v>205</v>
-      </c>
-      <c r="C29" s="176" t="s">
-        <v>288</v>
-      </c>
-      <c r="D29" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>283</v>
-      </c>
-      <c r="B30" s="171" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>175</v>
-      </c>
-      <c r="B31" s="171" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="177"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="176" t="s">
-        <v>260</v>
-      </c>
-      <c r="C33" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>263</v>
-      </c>
-      <c r="C37" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>266</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14029,7 +14077,7 @@
         <v>192</v>
       </c>
       <c r="C2" s="3">
-        <v>0.44900000000000001</v>
+        <v>0.43330000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -14039,157 +14087,427 @@
       <c r="B3" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>191</v>
-      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="124"/>
       <c r="B4" s="161" t="s">
-        <v>195</v>
+        <v>315</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>197</v>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="124"/>
+      <c r="B5" s="201" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>321</v>
+      </c>
+      <c r="D5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="126"/>
+      <c r="B6" s="172"/>
+      <c r="C6" s="163"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7" s="175" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="71"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="175" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="71"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="175" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="71"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="175" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="174" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="71"/>
+      <c r="E11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="174" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="174" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="71"/>
+      <c r="E13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="185" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="186" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="164" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="165"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="165" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="165"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="164" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="165"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="165" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="167"/>
+      <c r="D19" s="165"/>
+      <c r="E19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="162" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="73"/>
+      <c r="D20" s="165"/>
+      <c r="E20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="166" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="73"/>
+      <c r="D21" s="165"/>
+      <c r="E21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="162" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="73"/>
+      <c r="D22" s="165"/>
+      <c r="E22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="166" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="166"/>
+      <c r="D23" s="73"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="73"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="171" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" t="s">
+        <v>311</v>
+      </c>
+      <c r="D25" s="73"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="171" t="s">
+        <v>279</v>
+      </c>
+      <c r="D26" s="73"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="176"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="171" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="171" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="176" t="s">
+        <v>260</v>
+      </c>
+      <c r="C31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>263</v>
+      </c>
+      <c r="C35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="97" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="173">
+        <v>0.20619999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="161" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D4" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="124"/>
       <c r="B5" s="161" t="s">
-        <v>196</v>
+        <v>240</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="124"/>
       <c r="B6" s="161" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="124"/>
-      <c r="B7" s="161" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>189</v>
+        <v>305</v>
+      </c>
+      <c r="C6" s="163" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="126"/>
+      <c r="B7" s="201" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="200" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="126"/>
-      <c r="B8" s="172"/>
-      <c r="C8" s="163" t="s">
-        <v>251</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
+      <c r="B8" s="202"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="126"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32</v>
       </c>
-      <c r="B9" s="175" t="s">
+      <c r="B9" s="168" t="s">
         <v>228</v>
       </c>
-      <c r="C9" s="71" t="s">
-        <v>237</v>
-      </c>
-      <c r="D9" s="71" t="s">
-        <v>238</v>
-      </c>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
       <c r="E9" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="175" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" s="71" t="s">
-        <v>244</v>
-      </c>
-      <c r="D10" s="71" t="s">
-        <v>245</v>
-      </c>
+      <c r="B10" s="169" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="165" t="s">
+        <v>319</v>
+      </c>
+      <c r="D10" s="165"/>
       <c r="E10" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="175" t="s">
+      <c r="B11" s="168" t="s">
         <v>230</v>
       </c>
-      <c r="C11" s="71" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" s="71" t="s">
-        <v>250</v>
-      </c>
+      <c r="C11" s="165"/>
+      <c r="D11" s="165"/>
       <c r="E11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="175" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" s="71" t="s">
-        <v>182</v>
-      </c>
-      <c r="D12" s="71" t="s">
-        <v>245</v>
-      </c>
+      <c r="B12" s="169" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="165"/>
+      <c r="D12" s="165"/>
       <c r="E12" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="174" t="s">
+      <c r="B13" s="170" t="s">
         <v>232</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>259</v>
-      </c>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="174" t="s">
-        <v>247</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>257</v>
-      </c>
+      <c r="B14" s="171" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="174" t="s">
+      <c r="B15" s="170" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>255</v>
-      </c>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="185" t="s">
-        <v>248</v>
-      </c>
-      <c r="C16" s="186" t="s">
-        <v>252</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>253</v>
+      <c r="B16" s="171" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -14199,29 +14517,18 @@
       <c r="B18" s="164" t="s">
         <v>206</v>
       </c>
-      <c r="C18" s="165" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" s="165" t="s">
-        <v>213</v>
-      </c>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
       <c r="E18" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>178</v>
-      </c>
       <c r="B19" s="165" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="165" t="s">
-        <v>215</v>
-      </c>
-      <c r="D19" s="165" t="s">
-        <v>214</v>
-      </c>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
       <c r="E19" t="s">
         <v>217</v>
       </c>
@@ -14230,12 +14537,8 @@
       <c r="B20" s="164" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="165" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="165" t="s">
-        <v>211</v>
-      </c>
+      <c r="C20" s="165"/>
+      <c r="D20" s="165"/>
       <c r="E20" t="s">
         <v>218</v>
       </c>
@@ -14244,12 +14547,8 @@
       <c r="B21" s="165" t="s">
         <v>202</v>
       </c>
-      <c r="C21" s="167" t="s">
-        <v>200</v>
-      </c>
-      <c r="D21" s="165" t="s">
-        <v>201</v>
-      </c>
+      <c r="C21" s="165"/>
+      <c r="D21" s="165"/>
       <c r="E21" t="s">
         <v>219</v>
       </c>
@@ -14258,169 +14557,333 @@
       <c r="B22" s="162" t="s">
         <v>208</v>
       </c>
-      <c r="C22" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="D22" s="73" t="s">
-        <v>227</v>
-      </c>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="166" t="s">
         <v>204</v>
       </c>
-      <c r="C23" s="73" t="s">
-        <v>222</v>
-      </c>
-      <c r="D23" s="73" t="s">
-        <v>223</v>
-      </c>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="162" t="s">
         <v>209</v>
       </c>
-      <c r="C24" s="73" t="s">
-        <v>224</v>
-      </c>
-      <c r="D24" s="73" t="s">
-        <v>221</v>
-      </c>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="166" t="s">
         <v>205</v>
       </c>
-      <c r="C25" s="166" t="s">
-        <v>225</v>
-      </c>
-      <c r="D25" s="73" t="s">
-        <v>220</v>
+      <c r="C25" s="166"/>
+      <c r="D25" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="124" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="124"/>
+      <c r="B4" s="161" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="124"/>
+      <c r="B5" s="161" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="124"/>
+      <c r="B6" s="201" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>309</v>
+      </c>
+      <c r="D6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="126"/>
+      <c r="B7" s="172"/>
+      <c r="C7" s="163"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>32</v>
+      </c>
+      <c r="B8" s="175" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="175" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="175" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="175" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>297</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>298</v>
+      </c>
+      <c r="E11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="174" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="174" t="s">
+        <v>247</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="174" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="185" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" s="186" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="164" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="165"/>
+      <c r="D17" s="165"/>
+      <c r="E17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="165" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="164" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="165" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="167"/>
+      <c r="D20" s="165"/>
+      <c r="E20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="162" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="166" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="162" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="166" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="166"/>
+      <c r="D24" s="73"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="171" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" t="s">
+        <v>291</v>
+      </c>
+      <c r="D25" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>171</v>
-      </c>
       <c r="B26" s="171" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="D26" t="s">
-        <v>271</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="171" t="s">
-        <v>204</v>
-      </c>
-      <c r="C27" t="s">
-        <v>272</v>
-      </c>
-      <c r="D27" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>278</v>
+      </c>
       <c r="B28" s="171" t="s">
-        <v>280</v>
-      </c>
-      <c r="C28" t="s">
-        <v>275</v>
+        <v>205</v>
+      </c>
+      <c r="C28" s="176" t="s">
+        <v>287</v>
       </c>
       <c r="D28" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B29" s="171" t="s">
         <v>205</v>
       </c>
-      <c r="C29" s="176" t="s">
-        <v>277</v>
-      </c>
-      <c r="D29" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>283</v>
+        <v>175</v>
       </c>
       <c r="B30" s="171" t="s">
         <v>205</v>
       </c>
-      <c r="C30" t="s">
-        <v>281</v>
-      </c>
-      <c r="D30" t="s">
-        <v>282</v>
-      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>175</v>
-      </c>
-      <c r="B31" s="171" t="s">
-        <v>205</v>
-      </c>
-      <c r="C31" t="s">
-        <v>284</v>
-      </c>
+      <c r="B31" s="177"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>172</v>
-      </c>
-      <c r="B32" s="171" t="s">
-        <v>205</v>
-      </c>
-      <c r="C32" t="s">
-        <v>290</v>
-      </c>
-      <c r="D32" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="176" t="s">
+      <c r="B32" s="176" t="s">
         <v>260</v>
       </c>
-      <c r="C33" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>263</v>
-      </c>
-      <c r="C37" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>